<commit_message>
Notas que le colocamos a los compañeros
integrantes:
Miguel Daza
Heimis Miranda
</commit_message>
<xml_diff>
--- a/Notas.xlsx
+++ b/Notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimig\Desktop\ESPECIALIZACION - COHORTE 9\MODULO 4 - MODELOS Y ARQUITECTURA DE SOFTWARE\ENTREGAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407DCC44-3A14-4E2A-96DC-D544C2FA5B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E8A692-349D-4C47-B1DC-2926066265FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2900E099-2D5C-46F8-AC51-12FA74DCC6D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Evaluacion</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Victor Venegas</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A5691E-650E-4A9C-BE21-63F61C37F30C}">
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +507,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="1">
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D4" s="1">
         <v>4.7</v>
@@ -518,7 +521,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>4.3</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D5" s="1">
         <v>4.7</v>
@@ -534,7 +537,9 @@
       <c r="C6" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -544,9 +549,11 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>4.3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -556,9 +563,11 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>4.3</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -568,9 +577,11 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>4.3</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -582,7 +593,9 @@
       <c r="C10" s="1">
         <v>4</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -594,7 +607,9 @@
       <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -604,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="D12" s="1">
         <v>4.7</v>
@@ -618,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="D13" s="1">
         <v>4.7</v>
@@ -634,7 +649,9 @@
       <c r="C14" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>